<commit_message>
added old paper performances
</commit_message>
<xml_diff>
--- a/beagleUser/performances.xlsx
+++ b/beagleUser/performances.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10709"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcop/Desktop/marta/rna-division/beagleUser/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{EC7006FC-F505-1340-B126-C90B895EADFD}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21420" yWindow="3060" windowWidth="28800" windowHeight="17600" tabRatio="500"/>
+    <workbookView xWindow="12160" yWindow="3060" windowWidth="28800" windowHeight="17600" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150000"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>bear_orig</t>
   </si>
@@ -60,12 +61,18 @@
   </si>
   <si>
     <t>RRS</t>
+  </si>
+  <si>
+    <t>paper rnafold</t>
+  </si>
+  <si>
+    <t>paper curated</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -115,6 +122,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -382,140 +392,175 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="K1" s="1"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="C2" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="D2">
         <v>0.73699999999999999</v>
       </c>
-      <c r="C2">
+      <c r="E2">
         <v>0.58699999999999997</v>
       </c>
-      <c r="D2">
+      <c r="F2">
         <v>0.58499999999999996</v>
       </c>
-      <c r="E2">
+      <c r="G2">
         <v>0.61499999999999999</v>
       </c>
-      <c r="F2">
+      <c r="H2">
         <v>0.61299999999999999</v>
       </c>
-      <c r="G2">
+      <c r="I2">
         <v>0.627</v>
       </c>
-      <c r="H2">
+      <c r="J2">
         <v>0.626</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0.95</v>
+      </c>
+      <c r="D3">
         <v>0.751</v>
       </c>
-      <c r="C3">
+      <c r="E3">
         <v>0.75</v>
       </c>
-      <c r="D3">
+      <c r="F3">
         <v>0.75700000000000001</v>
       </c>
-      <c r="E3">
+      <c r="G3">
         <v>0.77500000000000002</v>
       </c>
-      <c r="F3">
+      <c r="H3">
         <v>0.77500000000000002</v>
       </c>
-      <c r="G3">
+      <c r="I3">
         <v>0.77459999999999996</v>
       </c>
-      <c r="H3">
+      <c r="J3">
         <v>0.77300000000000002</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0.95</v>
+      </c>
+      <c r="D4">
         <v>0.90600000000000003</v>
       </c>
-      <c r="C4">
+      <c r="E4">
         <v>0.91</v>
       </c>
-      <c r="D4">
+      <c r="F4">
         <v>0.91</v>
       </c>
-      <c r="E4">
+      <c r="G4">
         <v>0.91800000000000004</v>
-      </c>
-      <c r="F4">
-        <v>0.91800000000000004</v>
-      </c>
-      <c r="G4">
-        <v>0.91500000000000004</v>
       </c>
       <c r="H4">
         <v>0.91800000000000004</v>
       </c>
+      <c r="I4">
+        <v>0.91500000000000004</v>
+      </c>
+      <c r="J4">
+        <v>0.91800000000000004</v>
+      </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="D5">
         <v>0.64600000000000002</v>
       </c>
-      <c r="C5">
+      <c r="E5">
         <v>0.57399999999999995</v>
       </c>
-      <c r="D5">
+      <c r="F5">
         <v>0.57499999999999996</v>
       </c>
-      <c r="E5">
+      <c r="G5">
         <v>0.65200000000000002</v>
       </c>
-      <c r="F5">
+      <c r="H5">
         <v>0.65200000000000002</v>
       </c>
-      <c r="G5">
+      <c r="I5">
         <v>0.67200000000000004</v>
       </c>
-      <c r="H5">
+      <c r="J5">
         <v>0.67200000000000004</v>
       </c>
     </row>

</xml_diff>